<commit_message>
add some new image
</commit_message>
<xml_diff>
--- a/media/toa-do.xlsx
+++ b/media/toa-do.xlsx
@@ -195,9 +195,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -555,7 +555,7 @@
         <v>3490</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>645</v>
+        <v>700</v>
       </c>
       <c r="E30" s="3"/>
     </row>
@@ -567,7 +567,7 @@
         <v>3580</v>
       </c>
       <c r="C31" s="1" t="n">
-        <v>500</v>
+        <v>650</v>
       </c>
     </row>
   </sheetData>
@@ -594,7 +594,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -742,7 +742,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1297,7 +1297,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1348,7 +1348,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1399,7 +1399,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1450,7 +1450,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1528,7 +1528,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1606,7 +1606,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>